<commit_message>
Added first version of Indirect System
</commit_message>
<xml_diff>
--- a/gdr_features.xlsx
+++ b/gdr_features.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Все фичи</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Defered rendering</t>
+  </si>
+  <si>
+    <t>Формат задания сцены</t>
+  </si>
+  <si>
+    <t>Плагин для Blender</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,14 +531,14 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="5">
         <f>(COUNTA(B:B)-1)/(COUNTA(B:B)-1 +COUNTA(C:C)-1 ) * 100</f>
-        <v>61.53846153846154</v>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -543,7 +549,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
@@ -557,7 +563,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
@@ -571,21 +577,21 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>16</v>
@@ -614,7 +620,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -628,6 +634,9 @@
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D10" s="4" t="s">
         <v>21</v>
       </c>
@@ -636,6 +645,9 @@
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
@@ -714,6 +726,16 @@
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>